<commit_message>
Se logro el primero ❓
</commit_message>
<xml_diff>
--- a/Punto1Datos.xlsx
+++ b/Punto1Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Universidad de los Andes\College\8. Eighth Semester Stuff\Opti Avanzada IIND4101\Tarea1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Universidad de los Andes\College\8. Eighth Semester Stuff\Opti Avanzada IIND4101\Tarea1-IIND4101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75928EF4-AD64-4CBC-8474-8FFE24A48A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23636AC6-E0F2-4AF6-A80E-F576E936F762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ACAA2473-8227-4752-9AD6-AA96FDE0AF1C}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ACAA2473-8227-4752-9AD6-AA96FDE0AF1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Beneficios" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Ciencias</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Economía</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -569,10 +566,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD713244-99C9-4805-89D3-3E4BC98F6E74}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,8 +601,8 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>2.8</v>
@@ -627,11 +624,11 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+      <c r="B3">
+        <v>2.8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -650,14 +647,14 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
+      <c r="B4">
+        <v>1.7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
         <v>2.2999999999999998</v>
@@ -673,17 +670,17 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
+      <c r="B5">
+        <v>1.2</v>
+      </c>
+      <c r="C5">
+        <v>0.7</v>
+      </c>
+      <c r="D5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0.8</v>
@@ -696,23 +693,46 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
+      <c r="B6">
+        <v>0.9</v>
+      </c>
+      <c r="C6">
+        <v>0.6</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C7">
+        <v>3.1</v>
+      </c>
+      <c r="D7">
+        <v>1.7</v>
+      </c>
+      <c r="E7">
+        <v>0.9</v>
+      </c>
+      <c r="F7">
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -724,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0C2D40-D4A2-4021-9899-DC0579ECD09B}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +785,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
         <v>10</v>
       </c>
       <c r="C3">
@@ -782,11 +802,11 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
+      <c r="C4">
+        <v>11</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -799,14 +819,14 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
       </c>
       <c r="E5">
         <v>3</v>

</xml_diff>